<commit_message>
Pushing code for DriverScript, Util, config.properties
</commit_message>
<xml_diff>
--- a/Data Files/testdatasheet.xlsx
+++ b/Data Files/testdatasheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7190B5CB-B42C-41DB-A725-1A00008F1D94}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A8BED147-E899-470C-94ED-234DB1B2E7F5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>TCID</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>34</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -455,21 +464,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,78 +486,144 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -556,8 +631,9 @@
         <v>14</v>
       </c>
       <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -565,8 +641,9 @@
         <v>15</v>
       </c>
       <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -574,8 +651,9 @@
         <v>16</v>
       </c>
       <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -583,41 +661,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="4"/>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>